<commit_message>
refactor: ho fatto un casino
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferla\Documents\GitHub\MLPR-Fingerprint-Spoofing-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B11FB4A-A8C8-4550-9AA5-55EA4D2851F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A07A27-0FD4-4592-A8FD-4D10A49F523B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +71,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,7 +109,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>

</xml_diff>